<commit_message>
add S&P500 Symbol data
</commit_message>
<xml_diff>
--- a/Code/recommended_trades.xlsx
+++ b/Code/recommended_trades.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Ticker</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>ABBV</t>
+  </si>
+  <si>
+    <t>Market Captilization</t>
   </si>
 </sst>
 </file>
@@ -50,7 +53,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="$0.00"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,14 +64,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -115,14 +110,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,13 +424,13 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -447,13 +439,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2">
-        <v>127.62</v>
+        <v>126.05</v>
       </c>
       <c r="C2" s="2">
-        <v>37695885312</v>
+        <v>37232144384</v>
       </c>
       <c r="D2" s="3">
-        <v>1567</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -461,13 +453,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="2">
-        <v>17.42</v>
+        <v>16.79</v>
       </c>
       <c r="C3" s="2">
-        <v>11381565440</v>
+        <v>10969948160</v>
       </c>
       <c r="D3" s="3">
-        <v>11481</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -475,13 +467,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="2">
-        <v>70.73</v>
+        <v>73.17</v>
       </c>
       <c r="C4" s="2">
-        <v>4204467200</v>
+        <v>4349510144</v>
       </c>
       <c r="D4" s="3">
-        <v>2827</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -489,13 +481,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="2">
-        <v>191.94</v>
+        <v>195.83</v>
       </c>
       <c r="C5" s="2">
-        <v>3018966695936</v>
+        <v>3080151367680</v>
       </c>
       <c r="D5" s="3">
-        <v>1041</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -503,13 +495,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>143.74</v>
+        <v>150.85</v>
       </c>
       <c r="C6" s="2">
-        <v>253599055872</v>
+        <v>266143170560</v>
       </c>
       <c r="D6" s="3">
-        <v>1391</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
quantitative value strategy parameter and functions update
</commit_message>
<xml_diff>
--- a/Code/recommended_trades.xlsx
+++ b/Code/recommended_trades.xlsx
@@ -14,36 +14,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Ticker</t>
   </si>
   <si>
-    <t>Stock Price</t>
-  </si>
-  <si>
-    <t>Market Capitalization</t>
-  </si>
-  <si>
-    <t>Number of Shares to Buy</t>
+    <t>Current Price</t>
+  </si>
+  <si>
+    <t>Day High</t>
+  </si>
+  <si>
+    <t>Day Low</t>
+  </si>
+  <si>
+    <t>Previous Close</t>
+  </si>
+  <si>
+    <t>Trailing PE</t>
+  </si>
+  <si>
+    <t>Forward PE</t>
+  </si>
+  <si>
+    <t>PE Percentile</t>
+  </si>
+  <si>
+    <t>Price-to-Book Ratio</t>
+  </si>
+  <si>
+    <t>PB Percentile</t>
+  </si>
+  <si>
+    <t>Price-to-Sales Ratio</t>
+  </si>
+  <si>
+    <t>PS Percentile</t>
+  </si>
+  <si>
+    <t>EV/EBITDA</t>
+  </si>
+  <si>
+    <t>EV/EBITDA Percentile</t>
+  </si>
+  <si>
+    <t>EV/GP</t>
+  </si>
+  <si>
+    <t>EV/GP Percentile</t>
+  </si>
+  <si>
+    <t>RV Score</t>
   </si>
   <si>
     <t>A</t>
-  </si>
-  <si>
-    <t>AAL</t>
-  </si>
-  <si>
-    <t>AAP</t>
-  </si>
-  <si>
-    <t>AAPL</t>
-  </si>
-  <si>
-    <t>ABBV</t>
-  </si>
-  <si>
-    <t>Market Captilization</t>
   </si>
 </sst>
 </file>
@@ -53,7 +77,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="$0.00"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +88,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -110,11 +142,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -420,88 +455,110 @@
     <col min="4" max="4" width="18.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2">
         <v>126.05</v>
       </c>
       <c r="C2" s="2">
-        <v>37232144384</v>
+        <v>127.1</v>
       </c>
       <c r="D2" s="3">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2">
-        <v>16.79</v>
-      </c>
-      <c r="C3" s="2">
-        <v>10969948160</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1191</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2">
-        <v>73.17</v>
-      </c>
-      <c r="C4" s="2">
-        <v>4349510144</v>
-      </c>
-      <c r="D4" s="3">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2">
-        <v>195.83</v>
-      </c>
-      <c r="C5" s="2">
-        <v>3080151367680</v>
-      </c>
-      <c r="D5" s="3">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2">
-        <v>150.85</v>
-      </c>
-      <c r="C6" s="2">
-        <v>266143170560</v>
-      </c>
-      <c r="D6" s="3">
-        <v>132</v>
+        <v>123.16</v>
+      </c>
+      <c r="E2">
+        <v>126.66</v>
+      </c>
+      <c r="F2">
+        <v>27.825607</v>
+      </c>
+      <c r="G2">
+        <v>21.043407</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>6.43802</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>5.2886567</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>133169633206.8246</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>10.46429946910263</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>